<commit_message>
EWN: More changes after first full play
</commit_message>
<xml_diff>
--- a/CardFormatter/Data/EvenWithNougat/cards.datafile.xlsx
+++ b/CardFormatter/Data/EvenWithNougat/cards.datafile.xlsx
@@ -79,9 +79,6 @@
     <t xml:space="preserve">Discard a card. Draw a card. Rotate any 1 Equipment card. </t>
   </si>
   <si>
-    <t>Look at the top 2 cards of the deck. Activate an item on one of them.</t>
-  </si>
-  <si>
     <t>Reveal your plan. Either score it or activate an item on it.</t>
   </si>
   <si>
@@ -91,9 +88,6 @@
     <t>Swap any card with the Paradox. Your opponent may Discard a card then Draw a card.</t>
   </si>
   <si>
-    <t>Draw 2 cards. Return 2 of your Equipment cards.</t>
-  </si>
-  <si>
     <t>title</t>
   </si>
   <si>
@@ -133,21 +127,6 @@
     <t>s3</t>
   </si>
   <si>
-    <t>B: Play until you score every card from Era B and get at least 18 points during a single game, then pull the second sticker from the sleeve and apply its rules to the rule document.</t>
-  </si>
-  <si>
-    <t>8{+}:\nLook at the top 4 cards of the deck. Score or discard any number of them. Return the remainder in any order.</t>
-  </si>
-  <si>
-    <t>4{+}:\nDraw a card. Return or discard a card. Equip a card and activate it.</t>
-  </si>
-  <si>
-    <t>4{+}:\nAlways: When scoring treat this as any item.\nActivate: Rotate any number of equipment cards</t>
-  </si>
-  <si>
-    <t>Steal a fading card or a fragment.</t>
-  </si>
-  <si>
     <t>Biscuit</t>
   </si>
   <si>
@@ -220,54 +199,24 @@
     <t>{Era 2} get the {Biscuit} and the {Crowbar}!</t>
   </si>
   <si>
-    <t>B: Play until you score 16 points from cards in Era C during a single game, then pull the final sticker from the sleeve and apply its rules to the rule document.</t>
-  </si>
-  <si>
-    <t>C: Apply the Time Rift sticker to the card with the most {-} on it. Add 5{-} to the card. You may spend {+}{-} to change the name of an item on a card (which changes how it is scored).</t>
-  </si>
-  <si>
     <t>Time Rift\nIf this has more {-} than {+} and is played as an equipment card or revealed by the echo: erase it.</t>
   </si>
   <si>
-    <t>4{+}:\nDiscard a card. Draw 2 cards. Discard a card.</t>
-  </si>
-  <si>
-    <t>4{+}:\nAttach this as a tab to the edge of the card. While it is in the deck, at any time you may discard every card above this.</t>
-  </si>
-  <si>
-    <t>4{+}:\n Return 2 cards. Draw 4 cards. Discard or return 2 cards.</t>
-  </si>
-  <si>
     <t>4{+}:\nScore your plan for 2 points</t>
   </si>
   <si>
     <t>4{+}:\nLook at the entire deck and move 1 card in it to any position that you want.</t>
   </si>
   <si>
-    <t>4{+}:\n Draw 4 cards, return or discard 4 cards.</t>
-  </si>
-  <si>
     <t>4{+}:\n Look at the entire deck and either score a card from it, or keep a card from it. Discard or return a card.</t>
   </si>
   <si>
-    <t>8{+}:\n Always: you may activate 3 items a turn instead of 2.</t>
-  </si>
-  <si>
-    <t>4{+}:\nScore 1 of your Equipment cards as a fragment. Draw a card</t>
-  </si>
-  <si>
     <t>4{+}:\nConvert any card you have scored to be scored for 2 points.</t>
   </si>
   <si>
-    <t>4{+}:\n Look at up to 5 cards from the top of the deck. Return them in any order.</t>
-  </si>
-  <si>
     <t>4{+}:\n Either rotate any equipment card, or activate any item on one of your equipment.</t>
   </si>
   <si>
-    <t>4{+}:\nRotate, Score or Discard and repace the paradox.</t>
-  </si>
-  <si>
     <t>Daisies</t>
   </si>
   <si>
@@ -289,18 +238,9 @@
     <t>Fig Leaf.png</t>
   </si>
   <si>
-    <t>D:You may spend {+} to +1 a number on a card, or {+}{-}{-} to -1 a number on a card. You may spend {+}{+}{+} to mark on the back of a card where it starts the game (hand, paradox, num in deck, etc.).</t>
-  </si>
-  <si>
-    <t>A: After a game you may spend from a card the number of {+} on a mod sticker to apply it to the card (no covering other stickers). You may also spend {+} to mark the back of a card with 1 letter.</t>
-  </si>
-  <si>
     <t>Singularity\nWhen you have fewer than 25 points: If this card is scored or erased, instead the echo erases the paradox.</t>
   </si>
   <si>
-    <t>B: Apply the Singularity sticker to the other half of the card with the Time Rift on it. Add 5{-} to the card. Play until you score both the Singularity and 30+ points in a single game. Then you win.</t>
-  </si>
-  <si>
     <t>{Era 3} get the {Butterfly} and the {Stick Insect}!</t>
   </si>
   <si>
@@ -338,6 +278,66 @@
   </si>
   <si>
     <t>Discard a card. Look at the top 2 cards of the deck. Draw 1, Return or Discard the other.</t>
+  </si>
+  <si>
+    <t>3{+}:\nDraw a card. Return or discard a card. Equip a card and activate it.</t>
+  </si>
+  <si>
+    <t>3{+}:\nScore 1 of your Equipment cards as a fragment. Draw a card</t>
+  </si>
+  <si>
+    <t>3{+}:\nAlways: When scoring treat this as any item.\nActivate: Rotate any number of equipment cards</t>
+  </si>
+  <si>
+    <t>2{+}:\n Return 2 cards. Draw 4 cards. Discard or return 2 cards.</t>
+  </si>
+  <si>
+    <t>3{+}:\nRotate, Score, or Discard and repace the paradox.</t>
+  </si>
+  <si>
+    <t>3{+}:\n Look at up to 5 cards from the top of the deck. Return them in any order.</t>
+  </si>
+  <si>
+    <t>6{+}:\n Always: you may activate 3 items a turn instead of 2.</t>
+  </si>
+  <si>
+    <t>5{+}:\nLook at the top 4 cards of the deck. Score or discard any number of them. Return the remainder in any order.</t>
+  </si>
+  <si>
+    <t>A: Play until you score every card from Era B and get at least 18 points during a single game, then pull the second sticker from the sleeve and apply its rules to the rule document.</t>
+  </si>
+  <si>
+    <t>B: After a game you may spend from a card the number of {+} on a mod sticker to apply it to the card (no covering other stickers). You may also spend {+} to mark the back of a card with 1 letter.</t>
+  </si>
+  <si>
+    <t>A: Play until you score 16 points from cards in Era C during a single game, then pull the final sticker from the sleeve and apply its rules to the rule document.</t>
+  </si>
+  <si>
+    <t>Discard a card. Draw 2 cards. Discard a card.</t>
+  </si>
+  <si>
+    <t>2{+}:\nEither steal a fading card, or score a card normally.</t>
+  </si>
+  <si>
+    <t>Look at the top 2 cards of the deck. Activate an item on one of them. Return them.</t>
+  </si>
+  <si>
+    <t>Draw 2 cards. Return a card. Return one of your Equipment cards.</t>
+  </si>
+  <si>
+    <t>3{+}:\nAttach this as a tab to the edge of the card. While it is in the deck, at any time you may discard every card above this.</t>
+  </si>
+  <si>
+    <t>D:You may spend {+} to +1 a number on a card, or {+}{-}{-} to -1 a number on a card. You may spend {+}{+} to mark on the back of a card where it starts the game (hand, paradox, num in deck, etc.).</t>
+  </si>
+  <si>
+    <t>C: Apply the Time Rift sticker to the card with the most {-} on it. Add 4{-} to the card. You may spend {+}{-} to change the name of an item on a card (which changes how it is scored).</t>
+  </si>
+  <si>
+    <t>A: Apply the Singularity sticker to the other half of the card with the Time Rift on it. Add 4{-} to the card. Play until you score both the Singularity and 30+ points in a single game. Then you win.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3{+}:\n Draw 4 cards, return or discard 4 cards. Rotate any 1 Equipment card. </t>
   </si>
 </sst>
 </file>
@@ -1320,7 +1320,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1387,25 +1387,25 @@
         <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G2" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="H2" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="I2" t="s">
         <v>16</v>
       </c>
       <c r="J2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K2" t="s">
         <v>52</v>
-      </c>
-      <c r="K2" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1422,25 +1422,25 @@
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="F3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G3" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="H3" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="I3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K3" t="s">
         <v>53</v>
-      </c>
-      <c r="K3" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1457,25 +1457,25 @@
         <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G4" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="H4" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="I4" t="s">
         <v>18</v>
       </c>
       <c r="J4" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="K4" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1492,25 +1492,25 @@
         <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="F5" t="s">
         <v>16</v>
       </c>
       <c r="G5" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="H5" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="I5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J5" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="K5" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1527,25 +1527,25 @@
         <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="F6" t="s">
         <v>16</v>
       </c>
       <c r="G6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="H6" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="I6" t="s">
         <v>18</v>
       </c>
       <c r="J6" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="K6" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1562,25 +1562,25 @@
         <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G7" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="H7" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="I7" t="s">
         <v>18</v>
       </c>
       <c r="J7" t="s">
+        <v>50</v>
+      </c>
+      <c r="K7" t="s">
         <v>57</v>
-      </c>
-      <c r="K7" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1597,25 +1597,25 @@
         <v>13</v>
       </c>
       <c r="E8" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="F8" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="G8" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="H8" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="I8" t="s">
         <v>17</v>
       </c>
       <c r="J8" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="K8" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1632,25 +1632,25 @@
         <v>13</v>
       </c>
       <c r="E9" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="F9" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="G9" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="H9" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="I9" t="s">
         <v>15</v>
       </c>
       <c r="J9" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="K9" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1667,25 +1667,25 @@
         <v>13</v>
       </c>
       <c r="E10" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="F10" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="G10" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="H10" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="I10" t="s">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="J10" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="K10" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1702,25 +1702,25 @@
         <v>13</v>
       </c>
       <c r="E11" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="F11" t="s">
         <v>17</v>
       </c>
       <c r="G11" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="H11" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="I11" t="s">
         <v>15</v>
       </c>
       <c r="J11" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="K11" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1737,25 +1737,25 @@
         <v>13</v>
       </c>
       <c r="E12" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="F12" t="s">
         <v>17</v>
       </c>
       <c r="G12" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="H12" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="I12" t="s">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="J12" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="K12" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1772,25 +1772,25 @@
         <v>13</v>
       </c>
       <c r="E13" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="F13" t="s">
         <v>15</v>
       </c>
       <c r="G13" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H13" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="I13" t="s">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="J13" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="K13" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1807,25 +1807,25 @@
         <v>14</v>
       </c>
       <c r="E14" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="F14" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="G14" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="H14" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="I14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J14" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="K14" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1842,25 +1842,25 @@
         <v>14</v>
       </c>
       <c r="E15" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="F15" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="G15" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="H15" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="I15" t="s">
-        <v>41</v>
+        <v>97</v>
       </c>
       <c r="J15" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="K15" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1877,25 +1877,25 @@
         <v>14</v>
       </c>
       <c r="E16" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="F16" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="G16" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="H16" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="I16" t="s">
-        <v>23</v>
+        <v>100</v>
       </c>
       <c r="J16" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="K16" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1912,25 +1912,25 @@
         <v>14</v>
       </c>
       <c r="E17" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="F17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G17" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="H17" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="I17" t="s">
-        <v>41</v>
+        <v>97</v>
       </c>
       <c r="J17" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="K17" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -1947,25 +1947,25 @@
         <v>14</v>
       </c>
       <c r="E18" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="F18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G18" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="H18" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="I18" t="s">
-        <v>23</v>
+        <v>100</v>
       </c>
       <c r="J18" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="K18" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1982,25 +1982,25 @@
         <v>14</v>
       </c>
       <c r="E19" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="F19" t="s">
-        <v>41</v>
+        <v>97</v>
       </c>
       <c r="G19" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="H19" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="I19" t="s">
-        <v>23</v>
+        <v>100</v>
       </c>
       <c r="J19" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="K19" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -2017,7 +2017,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2045,31 +2045,31 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="M1" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="4" customFormat="1" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2077,40 +2077,40 @@
         <v>19</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E2" s="3">
         <v>1</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>39</v>
+        <v>86</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>70</v>
+        <v>101</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>69</v>
+        <v>98</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>40</v>
+        <v>88</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>37</v>
+        <v>94</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="4" customFormat="1" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2118,40 +2118,40 @@
         <v>20</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E3" s="4">
         <v>2</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>71</v>
+        <v>89</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>66</v>
+        <v>96</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>67</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:13" s="4" customFormat="1" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2159,40 +2159,40 @@
         <v>21</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E4" s="4">
         <v>3</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>38</v>
+        <v>93</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>74</v>
+        <v>105</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>